<commit_message>
Site updated: 2022-08-06 21:33:46
</commit_message>
<xml_diff>
--- a/2022/08/06/Python-DS-111-1001commit/질문정리.xlsx
+++ b/2022/08/06/Python-DS-111-1001commit/질문정리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeitplatz\03_blog\source\_posts\Python-DS-111-1001commit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{665C54D7-1C4E-42D2-8B3D-F8143E547F17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CAFD5E-4763-4188-9BFB-575BA16E610B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" xr2:uid="{07929FDA-E429-4E58-BFEA-ABDE1F132C1D}"/>
   </bookViews>
@@ -25,32 +25,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
+  <si>
+    <t>1. github 관련</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-1. repository 관련</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공개 가능한지?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제가 어떤 것들인지?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>iilii</t>
-  </si>
-  <si>
-    <t>1. github 관련</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-1. repository 관련</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>공개 가능한지?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>주제가 어떤 것들인지?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>iilii</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>나도 만들어서 해보고 싶다. 팁을 주신다면?</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -193,10 +186,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>주로 커밋하는 내용</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>지금 하는 일</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -265,10 +254,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>안세홋</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>천일커밋을 하려는 후배들에게 주고 싶은 팁</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -289,10 +274,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>목승찬, 손성민, 우왕</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>천일커밋 동기, 계기, 원동력</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -394,10 +375,6 @@
   </si>
   <si>
     <t>가족들의 반응은?, 300일-600일-900일 되었을 때 주변 반응은?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>iilii, 우왕, 코쟁이</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -440,6 +417,14 @@
   </si>
   <si>
     <t>하루 일과는 어떤지. 얼마나 규칙적으로 일과를 유지하는지., 회사일과 개인 배움과 성장, 가정에서의 역할을 어떻게 균형있게 하고 있는지. 한쪽이 소홀해서 개선이 필요하다고 생각되는 부분이 있는지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>iilii, 우왕, 코쟁이, 목승찬, 손성민</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>iilii, 안세홋</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -477,12 +462,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -499,11 +490,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -818,156 +812,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD28965-89D5-4132-807A-0B8B66E8EDF7}">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
+      <c r="D15" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>7</v>
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
         <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -975,194 +971,257 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
       <c r="D34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D45" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="D46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
-        <v>41</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="D60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>38</v>
-      </c>
-      <c r="D57" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
-        <v>84</v>
-      </c>
-      <c r="D58" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
-        <v>31</v>
-      </c>
-      <c r="D59" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
-        <v>33</v>
-      </c>
-      <c r="D60" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C61" t="s">
-        <v>35</v>
-      </c>
-      <c r="D61" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
-        <v>39</v>
-      </c>
-      <c r="D62" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
-        <v>52</v>
-      </c>
       <c r="D63" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D64" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
-        <v>64</v>
-      </c>
-      <c r="D65" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
-        <v>70</v>
-      </c>
-      <c r="D66" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="D67" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>58</v>
+      </c>
+      <c r="D68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
         <v>82</v>
       </c>
@@ -1170,98 +1229,17 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C76" t="s">
-        <v>97</v>
-      </c>
-      <c r="D76" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C77" t="s">
-        <v>74</v>
-      </c>
-      <c r="D77" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C81" t="s">
-        <v>46</v>
-      </c>
-      <c r="D81" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C82" t="s">
-        <v>46</v>
-      </c>
-      <c r="D82" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C85" t="s">
-        <v>50</v>
-      </c>
-      <c r="D85" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C86" t="s">
-        <v>62</v>
-      </c>
-      <c r="D86" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B88" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C89" t="s">
-        <v>87</v>
-      </c>
-      <c r="D89" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B91" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C92" t="s">
-        <v>76</v>
-      </c>
-      <c r="D92" t="s">
-        <v>77</v>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>71</v>
+      </c>
+      <c r="D74" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>